<commit_message>
added jupyter notebook file
</commit_message>
<xml_diff>
--- a/correlation.xlsx
+++ b/correlation.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Uros\Desktop\Fertility\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Uros\Desktop\Fertility\code\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9384"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="16">
   <si>
     <t>Season in which the analysis was performed</t>
   </si>
@@ -66,6 +66,12 @@
   </si>
   <si>
     <t>Chi square (X^2) test with respect to Output value</t>
+  </si>
+  <si>
+    <t>pca, decision tree - da se vidi koje su promenljive upotrebljene pri korenu</t>
+  </si>
+  <si>
+    <t>data augmentation</t>
   </si>
 </sst>
 </file>
@@ -392,15 +398,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S12"/>
+  <dimension ref="A1:V12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+      <selection activeCell="V3" sqref="V3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>11</v>
       </c>
@@ -422,7 +428,7 @@
       <c r="R1" s="3"/>
       <c r="S1" s="3"/>
     </row>
-    <row r="2" spans="1:19" ht="105" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -462,8 +468,11 @@
       <c r="P2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="3" spans="1:19" ht="105" x14ac:dyDescent="0.25">
+      <c r="V2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -503,8 +512,11 @@
       <c r="P3" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:19" ht="75" x14ac:dyDescent="0.25">
+      <c r="V3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" ht="72" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
@@ -545,7 +557,7 @@
         <v>3.0460495288398099E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:22" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
@@ -586,7 +598,7 @@
         <v>7.5242574065559498E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:19" ht="60" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:22" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -627,7 +639,7 @@
         <v>7.92290639796389E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:19" ht="60" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:22" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
@@ -668,7 +680,7 @@
         <v>0.105158004848391</v>
       </c>
     </row>
-    <row r="8" spans="1:19" ht="75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:22" ht="72" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
@@ -709,7 +721,7 @@
         <v>0.221355866573897</v>
       </c>
     </row>
-    <row r="9" spans="1:19" ht="105" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:22" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
@@ -750,7 +762,7 @@
         <v>0.22908845532880501</v>
       </c>
     </row>
-    <row r="10" spans="1:19" ht="75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:22" ht="72" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
@@ -791,7 +803,7 @@
         <v>0.54584462801423395</v>
       </c>
     </row>
-    <row r="11" spans="1:19" ht="75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:22" ht="72" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>8</v>
       </c>
@@ -832,7 +844,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>9</v>
       </c>

</xml_diff>